<commit_message>
Added star information in plantary info spreadsheet
</commit_message>
<xml_diff>
--- a/docs/planets.xlsx
+++ b/docs/planets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TA048699\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Git\website\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="5688"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="5685"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>Kaihl</t>
   </si>
@@ -138,6 +138,18 @@
   </si>
   <si>
     <t>Newly Livable thanks to an man-made atmosphere</t>
+  </si>
+  <si>
+    <t>Io</t>
+  </si>
+  <si>
+    <t>Asgorath</t>
+  </si>
+  <si>
+    <t>Star</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
@@ -493,20 +505,20 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
-    <col min="6" max="6" width="42.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -526,17 +538,35 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
       <c r="E2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
       <c r="E3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -550,7 +580,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -564,7 +594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -581,7 +611,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -601,7 +631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -618,7 +648,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -632,7 +662,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -649,7 +679,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -666,7 +696,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -683,7 +713,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -700,7 +730,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -717,7 +747,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -736,5 +766,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added updates to planets and starships spreadsheets
</commit_message>
<xml_diff>
--- a/docs/planets.xlsx
+++ b/docs/planets.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="5685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="5688"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -505,20 +505,20 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="42.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="42.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -538,7 +538,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -552,7 +552,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -566,7 +566,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -580,7 +580,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -594,7 +594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -611,7 +611,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -631,7 +631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -648,7 +648,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -662,7 +662,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -679,7 +679,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -696,7 +696,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -713,7 +713,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -730,12 +730,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -747,7 +747,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>

</xml_diff>